<commit_message>
update parts 4 and 5, deleted Rproject
</commit_message>
<xml_diff>
--- a/Presentations/psoriasis.xlsx
+++ b/Presentations/psoriasis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kgx936/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kgx936/Desktop/FromExceltoR/Presentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BF9F89-AC6D-B14B-B7F0-45AF25E08335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF7495D-3E47-1F4E-A17A-942EBB9AA9DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>GeneA</t>
+  </si>
+  <si>
+    <t>GeneB</t>
+  </si>
+  <si>
+    <t>GeneC</t>
+  </si>
+  <si>
+    <t>GeneD</t>
+  </si>
+  <si>
+    <t>GeneE</t>
+  </si>
+  <si>
+    <t>GeneF</t>
+  </si>
+  <si>
+    <t>GeneG</t>
+  </si>
+  <si>
+    <t>GeneH</t>
+  </si>
+  <si>
+    <t>GeneI</t>
+  </si>
+  <si>
+    <t>GeneJ</t>
   </si>
   <si>
     <t>psne</t>
@@ -421,316 +451,1456 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>0.84090909999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>2.943064468213505</v>
+      </c>
+      <c r="D2">
+        <v>3.1614498348652882</v>
+      </c>
+      <c r="E2">
+        <v>4.2135343127013343</v>
+      </c>
+      <c r="F2">
+        <v>-0.47592158467205109</v>
+      </c>
+      <c r="G2">
+        <v>4.2022900156703109</v>
+      </c>
+      <c r="H2">
+        <v>0.33471741586850251</v>
+      </c>
+      <c r="I2">
+        <v>5.2007993698567079</v>
+      </c>
+      <c r="J2">
+        <v>0.1668755111514782</v>
+      </c>
+      <c r="K2">
+        <v>1.998720997616684</v>
+      </c>
+      <c r="L2">
+        <v>4.6234983311909827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0.95454550000000005</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2.6717805189095669</v>
+      </c>
+      <c r="D3">
+        <v>3.2282606324884271</v>
+      </c>
+      <c r="E3">
+        <v>6.087297819679474</v>
+      </c>
+      <c r="F3">
+        <v>0.1211229011149285</v>
+      </c>
+      <c r="G3">
+        <v>3.6625961897538599</v>
+      </c>
+      <c r="H3">
+        <v>1.2766676996042861</v>
+      </c>
+      <c r="I3">
+        <v>5.5159888287153072</v>
+      </c>
+      <c r="J3">
+        <v>5.8038410138726182E-2</v>
+      </c>
+      <c r="K3">
+        <v>2.0555758255435741</v>
+      </c>
+      <c r="L3">
+        <v>4.3484517424784279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>1.0681818000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>2.527458673996672</v>
+      </c>
+      <c r="D4">
+        <v>2.7958557367676491</v>
+      </c>
+      <c r="E4">
+        <v>4.4800980902291236</v>
+      </c>
+      <c r="F4">
+        <v>-0.16531141996051751</v>
+      </c>
+      <c r="G4">
+        <v>3.90108296325106</v>
+      </c>
+      <c r="H4">
+        <v>1.1804869834949141</v>
+      </c>
+      <c r="I4">
+        <v>5.4025107567883817</v>
+      </c>
+      <c r="J4">
+        <v>-0.20223273339542999</v>
+      </c>
+      <c r="K4">
+        <v>1.945153952007227</v>
+      </c>
+      <c r="L4">
+        <v>2.5667267111798679</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>1.1136364000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>3.5596605968768911</v>
+      </c>
+      <c r="D5">
+        <v>2.5316484573529481</v>
+      </c>
+      <c r="E5">
+        <v>4.9650462876805648</v>
+      </c>
+      <c r="F5">
+        <v>0.13878689971868249</v>
+      </c>
+      <c r="G5">
+        <v>2.9224703850715148</v>
+      </c>
+      <c r="H5">
+        <v>0.74384484731456557</v>
+      </c>
+      <c r="I5">
+        <v>4.9822579257183746</v>
+      </c>
+      <c r="J5">
+        <v>-0.32850259942616278</v>
+      </c>
+      <c r="K5">
+        <v>2.0286638127595831</v>
+      </c>
+      <c r="L5">
+        <v>3.165982145138897</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>1.1818181999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>3.4829229135966089</v>
+      </c>
+      <c r="D6">
+        <v>2.79272088952641</v>
+      </c>
+      <c r="E6">
+        <v>4.7397755181479084</v>
+      </c>
+      <c r="F6">
+        <v>-0.1019917660498787</v>
+      </c>
+      <c r="G6">
+        <v>3.043419838512301</v>
+      </c>
+      <c r="H6">
+        <v>0.51265511772629258</v>
+      </c>
+      <c r="I6">
+        <v>5.4751229341401606</v>
+      </c>
+      <c r="J6">
+        <v>-0.1163384285130785</v>
+      </c>
+      <c r="K6">
+        <v>2.0440871684112429</v>
+      </c>
+      <c r="L6">
+        <v>3.6077271939292719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1.2045455</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>2.9377554181244951</v>
+      </c>
+      <c r="D7">
+        <v>3.1239786592015708</v>
+      </c>
+      <c r="E7">
+        <v>4.1973632467486484</v>
+      </c>
+      <c r="F7">
+        <v>-0.20030259950313609</v>
+      </c>
+      <c r="G7">
+        <v>3.458246508696766</v>
+      </c>
+      <c r="H7">
+        <v>0.4723984168633234</v>
+      </c>
+      <c r="I7">
+        <v>3.947422432165506</v>
+      </c>
+      <c r="J7">
+        <v>-0.12889459115738361</v>
+      </c>
+      <c r="K7">
+        <v>1.5509692107360209</v>
+      </c>
+      <c r="L7">
+        <v>3.5608288385605311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1.3181818000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>2.609418556267328</v>
+      </c>
+      <c r="D8">
+        <v>3.0791955643791691</v>
+      </c>
+      <c r="E8">
+        <v>5.6400563391372556</v>
+      </c>
+      <c r="F8">
+        <v>-0.13686149451336241</v>
+      </c>
+      <c r="G8">
+        <v>3.9747501493780688</v>
+      </c>
+      <c r="H8">
+        <v>1.0290442330257989</v>
+      </c>
+      <c r="I8">
+        <v>4.9154575619206176</v>
+      </c>
+      <c r="J8">
+        <v>0.42933692644596289</v>
+      </c>
+      <c r="K8">
+        <v>1.743615153617627</v>
+      </c>
+      <c r="L8">
+        <v>3.523011516386378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1.2954545</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>2.776942136203242</v>
+      </c>
+      <c r="D9">
+        <v>2.8985285228654378</v>
+      </c>
+      <c r="E9">
+        <v>4.8689638221688494</v>
+      </c>
+      <c r="F9">
+        <v>7.6452850503897926E-2</v>
+      </c>
+      <c r="G9">
+        <v>3.4352549682759279</v>
+      </c>
+      <c r="H9">
+        <v>1.3477094316245199</v>
+      </c>
+      <c r="I9">
+        <v>5.5595578986038916</v>
+      </c>
+      <c r="J9">
+        <v>-7.7574091742740103E-2</v>
+      </c>
+      <c r="K9">
+        <v>1.51197801769833</v>
+      </c>
+      <c r="L9">
+        <v>3.1793215481943911</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>1.3863635999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>2.8910311186080562</v>
+      </c>
+      <c r="D10">
+        <v>2.7653837969970501</v>
+      </c>
+      <c r="E10">
+        <v>5.4735523513734341</v>
+      </c>
+      <c r="F10">
+        <v>-3.3070222599825713E-2</v>
+      </c>
+      <c r="G10">
+        <v>3.3465891850384981</v>
+      </c>
+      <c r="H10">
+        <v>1.1724248956063581</v>
+      </c>
+      <c r="I10">
+        <v>4.4142062799600366</v>
+      </c>
+      <c r="J10">
+        <v>0.18410440008469969</v>
+      </c>
+      <c r="K10">
+        <v>1.813413962587382</v>
+      </c>
+      <c r="L10">
+        <v>4.0216152946109789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1.4090909</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>2.9740054514333489</v>
+      </c>
+      <c r="D11">
+        <v>3.0316547154715869</v>
+      </c>
+      <c r="E11">
+        <v>5.1518455591741059</v>
+      </c>
+      <c r="F11">
+        <v>-0.16082048801882581</v>
+      </c>
+      <c r="G11">
+        <v>4.2127106211810332</v>
+      </c>
+      <c r="H11">
+        <v>1.1191013350390591</v>
+      </c>
+      <c r="I11">
+        <v>5.3006583820241824</v>
+      </c>
+      <c r="J11">
+        <v>-0.23217967431216219</v>
+      </c>
+      <c r="K11">
+        <v>2.016539012869679</v>
+      </c>
+      <c r="L11">
+        <v>3.713031242262844</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>1.5454545</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>3.4803413466227111</v>
+      </c>
+      <c r="D12">
+        <v>3.0596495170333902</v>
+      </c>
+      <c r="E12">
+        <v>3.1897891557408218</v>
+      </c>
+      <c r="F12">
+        <v>0.35054222512864558</v>
+      </c>
+      <c r="G12">
+        <v>2.594716183040513</v>
+      </c>
+      <c r="H12">
+        <v>0.63355536422288761</v>
+      </c>
+      <c r="I12">
+        <v>4.5712897405684298</v>
+      </c>
+      <c r="J12">
+        <v>-0.61544415704945332</v>
+      </c>
+      <c r="K12">
+        <v>1.990110316833767</v>
+      </c>
+      <c r="L12">
+        <v>3.1793018746749868</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1.6363635999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>2.9521587597510819</v>
+      </c>
+      <c r="D13">
+        <v>2.991881705908384</v>
+      </c>
+      <c r="E13">
+        <v>5.0103599426108296</v>
+      </c>
+      <c r="F13">
+        <v>0.19081662057315851</v>
+      </c>
+      <c r="G13">
+        <v>3.323657529388643</v>
+      </c>
+      <c r="H13">
+        <v>1.276581308299253</v>
+      </c>
+      <c r="I13">
+        <v>5.2016662028526319</v>
+      </c>
+      <c r="J13">
+        <v>-0.13582871525040599</v>
+      </c>
+      <c r="K13">
+        <v>1.955058509659531</v>
+      </c>
+      <c r="L13">
+        <v>3.0955414430824559</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>1.8181818000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>2.8651772860081821</v>
+      </c>
+      <c r="D14">
+        <v>2.814865598612823</v>
+      </c>
+      <c r="E14">
+        <v>4.2240974360335644</v>
+      </c>
+      <c r="F14">
+        <v>-8.4044371955900865E-2</v>
+      </c>
+      <c r="G14">
+        <v>3.6702002515710519</v>
+      </c>
+      <c r="H14">
+        <v>1.0063503566614671</v>
+      </c>
+      <c r="I14">
+        <v>4.9065883254621001</v>
+      </c>
+      <c r="J14">
+        <v>-0.21243913685193069</v>
+      </c>
+      <c r="K14">
+        <v>1.750964173460748</v>
+      </c>
+      <c r="L14">
+        <v>3.4809556564457629</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>1.9545455</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>2.630888559980693</v>
+      </c>
+      <c r="D15">
+        <v>2.6429005427721171</v>
+      </c>
+      <c r="E15">
+        <v>4.7919908231564223</v>
+      </c>
+      <c r="F15">
+        <v>-1.808436600156391E-3</v>
+      </c>
+      <c r="G15">
+        <v>4.1855586108397409</v>
+      </c>
+      <c r="H15">
+        <v>1.460774003613786</v>
+      </c>
+      <c r="I15">
+        <v>4.4129037287651309</v>
+      </c>
+      <c r="J15">
+        <v>-5.3189704656247602E-2</v>
+      </c>
+      <c r="K15">
+        <v>2.156251074892571</v>
+      </c>
+      <c r="L15">
+        <v>4.1384649543235206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>2.0909091000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>3.4312977139014489</v>
+      </c>
+      <c r="D16">
+        <v>3.163797244172327</v>
+      </c>
+      <c r="E16">
+        <v>4.4074099215134828</v>
+      </c>
+      <c r="F16">
+        <v>4.4978637210072933E-2</v>
+      </c>
+      <c r="G16">
+        <v>2.4681284069331419</v>
+      </c>
+      <c r="H16">
+        <v>1.178984577481099</v>
+      </c>
+      <c r="I16">
+        <v>4.2692719649026261</v>
+      </c>
+      <c r="J16">
+        <v>0.17580512933894249</v>
+      </c>
+      <c r="K16">
+        <v>2.0429219268707821</v>
+      </c>
+      <c r="L16">
+        <v>3.9623615061206112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>0.59090909999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>0.113505665975432</v>
+      </c>
+      <c r="D17">
+        <v>6.9172880792285776</v>
+      </c>
+      <c r="E17">
+        <v>-0.1600356259922337</v>
+      </c>
+      <c r="F17">
+        <v>0.89570809482710523</v>
+      </c>
+      <c r="G17">
+        <v>3.7002664742610851</v>
+      </c>
+      <c r="H17">
+        <v>7.7021167091747236E-2</v>
+      </c>
+      <c r="I17">
+        <v>6.8185398874668417</v>
+      </c>
+      <c r="J17">
+        <v>1.039623978297916</v>
+      </c>
+      <c r="K17">
+        <v>4.4467787668344769</v>
+      </c>
+      <c r="L17">
+        <v>3.8500625945762801</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>0.68181820000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>0.36612679097637291</v>
+      </c>
+      <c r="D18">
+        <v>6.8756583822130963</v>
+      </c>
+      <c r="E18">
+        <v>-0.49731295735477238</v>
+      </c>
+      <c r="F18">
+        <v>1.0925409848066741</v>
+      </c>
+      <c r="G18">
+        <v>3.1140270554128242</v>
+      </c>
+      <c r="H18">
+        <v>-0.10677376825839111</v>
+      </c>
+      <c r="I18">
+        <v>7.2160913363973354</v>
+      </c>
+      <c r="J18">
+        <v>1.3066297683367141</v>
+      </c>
+      <c r="K18">
+        <v>4.8852276880437726</v>
+      </c>
+      <c r="L18">
+        <v>3.889729387386379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>0.72727269999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>6.0698914324775713E-2</v>
+      </c>
+      <c r="D19">
+        <v>5.4836632168183508</v>
+      </c>
+      <c r="E19">
+        <v>6.5800770848433221E-2</v>
+      </c>
+      <c r="F19">
+        <v>1.102213837176053</v>
+      </c>
+      <c r="G19">
+        <v>2.422383091747129</v>
+      </c>
+      <c r="H19">
+        <v>-0.2370309973586284</v>
+      </c>
+      <c r="I19">
+        <v>7.1845191488364408</v>
+      </c>
+      <c r="J19">
+        <v>0.77453825838838242</v>
+      </c>
+      <c r="K19">
+        <v>4.9700295551805764</v>
+      </c>
+      <c r="L19">
+        <v>3.543959835779428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>6.6092165691767762E-2</v>
+      </c>
+      <c r="D20">
+        <v>7.1372412665056739</v>
+      </c>
+      <c r="E20">
+        <v>9.1296804304691559E-2</v>
+      </c>
+      <c r="F20">
+        <v>1.2054569174188969</v>
+      </c>
+      <c r="G20">
+        <v>2.8242426778856999</v>
+      </c>
+      <c r="H20">
+        <v>-0.56813659269443317</v>
+      </c>
+      <c r="I20">
+        <v>6.2481872379931964</v>
+      </c>
+      <c r="J20">
+        <v>1.1344170159001641</v>
+      </c>
+      <c r="K20">
+        <v>5.0074601306252804</v>
+      </c>
+      <c r="L20">
+        <v>3.311743105387793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>0.73636360000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>0.14715393702071539</v>
+      </c>
+      <c r="D21">
+        <v>7.5562266142186783</v>
+      </c>
+      <c r="E21">
+        <v>-7.6841320115863324E-2</v>
+      </c>
+      <c r="F21">
+        <v>1.0369098182153831</v>
+      </c>
+      <c r="G21">
+        <v>2.3123035996513228</v>
+      </c>
+      <c r="H21">
+        <v>0.73625775420181427</v>
+      </c>
+      <c r="I21">
+        <v>8.0980216478136704</v>
+      </c>
+      <c r="J21">
+        <v>0.92807060655249063</v>
+      </c>
+      <c r="K21">
+        <v>4.4426667195062084</v>
+      </c>
+      <c r="L21">
+        <v>3.153366797384789</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B22">
         <v>0.81818179999999996</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>4.0997656105049282E-2</v>
+      </c>
+      <c r="D22">
+        <v>6.3392198916775424</v>
+      </c>
+      <c r="E22">
+        <v>-0.1265950009663338</v>
+      </c>
+      <c r="F22">
+        <v>0.92034570203056076</v>
+      </c>
+      <c r="G22">
+        <v>3.4371464684953388</v>
+      </c>
+      <c r="H22">
+        <v>1.064801840766473</v>
+      </c>
+      <c r="I22">
+        <v>6.9841290499762554</v>
+      </c>
+      <c r="J22">
+        <v>0.24589652469061099</v>
+      </c>
+      <c r="K22">
+        <v>5.1654003233962413</v>
+      </c>
+      <c r="L22">
+        <v>3.394998774124268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>0.86363639999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>1.1134585636877641</v>
+      </c>
+      <c r="D23">
+        <v>7.1841836644453956</v>
+      </c>
+      <c r="E23">
+        <v>-4.6666270359444831E-2</v>
+      </c>
+      <c r="F23">
+        <v>1.078743383944609</v>
+      </c>
+      <c r="G23">
+        <v>3.8140745478744211</v>
+      </c>
+      <c r="H23">
+        <v>0.47086667951753403</v>
+      </c>
+      <c r="I23">
+        <v>7.1231266618131093</v>
+      </c>
+      <c r="J23">
+        <v>1.2130104518636691</v>
+      </c>
+      <c r="K23">
+        <v>5.8318104803004038</v>
+      </c>
+      <c r="L23">
+        <v>3.6145221457584098</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B24">
         <v>0.93181820000000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>-0.27223873792107489</v>
+      </c>
+      <c r="D24">
+        <v>7.0219408873242717</v>
+      </c>
+      <c r="E24">
+        <v>0.24256383001422019</v>
+      </c>
+      <c r="F24">
+        <v>0.7992747429216972</v>
+      </c>
+      <c r="G24">
+        <v>3.270111760406504</v>
+      </c>
+      <c r="H24">
+        <v>0.21641543834421131</v>
+      </c>
+      <c r="I24">
+        <v>6.1211342545564253</v>
+      </c>
+      <c r="J24">
+        <v>1.150153321025823</v>
+      </c>
+      <c r="K24">
+        <v>5.478734642193686</v>
+      </c>
+      <c r="L24">
+        <v>3.5891096795003818</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>0.90909090000000004</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>0.39160323706916972</v>
+      </c>
+      <c r="D25">
+        <v>6.1951790275084813</v>
+      </c>
+      <c r="E25">
+        <v>9.7639738396759088E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.61192714300922035</v>
+      </c>
+      <c r="G25">
+        <v>3.7013505491833492</v>
+      </c>
+      <c r="H25">
+        <v>0.28791710996602321</v>
+      </c>
+      <c r="I25">
+        <v>7.0718054516740754</v>
+      </c>
+      <c r="J25">
+        <v>0.71091638075104502</v>
+      </c>
+      <c r="K25">
+        <v>4.9138259241077291</v>
+      </c>
+      <c r="L25">
+        <v>3.4158091911797022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B26">
         <v>0.95454550000000005</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>-0.12861999788555359</v>
+      </c>
+      <c r="D26">
+        <v>7.0013898785361972</v>
+      </c>
+      <c r="E26">
+        <v>0.29461389674137972</v>
+      </c>
+      <c r="F26">
+        <v>1.287354254405304</v>
+      </c>
+      <c r="G26">
+        <v>3.7270627526176652</v>
+      </c>
+      <c r="H26">
+        <v>-0.55951579591938483</v>
+      </c>
+      <c r="I26">
+        <v>6.7258335205796183</v>
+      </c>
+      <c r="J26">
+        <v>1.054775763724489</v>
+      </c>
+      <c r="K26">
+        <v>5.3888943232300246</v>
+      </c>
+      <c r="L26">
+        <v>4.946302266140588</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B27">
         <v>1.1590909</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>-9.84802673189836E-2</v>
+      </c>
+      <c r="D27">
+        <v>9.2470292599749229</v>
+      </c>
+      <c r="E27">
+        <v>-0.43305305609885458</v>
+      </c>
+      <c r="F27">
+        <v>1.2211559702012851</v>
+      </c>
+      <c r="G27">
+        <v>1.9557861706224999</v>
+      </c>
+      <c r="H27">
+        <v>-0.35167905360621188</v>
+      </c>
+      <c r="I27">
+        <v>8.1893955840190085</v>
+      </c>
+      <c r="J27">
+        <v>1.167938890259473</v>
+      </c>
+      <c r="K27">
+        <v>5.4322776088567402</v>
+      </c>
+      <c r="L27">
+        <v>3.9525971538344411</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B28">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>-0.18370149224913859</v>
+      </c>
+      <c r="D28">
+        <v>7.0669227300068451</v>
+      </c>
+      <c r="E28">
+        <v>-5.4656768816519617E-2</v>
+      </c>
+      <c r="F28">
+        <v>1.109459320133132</v>
+      </c>
+      <c r="G28">
+        <v>2.7309636050064579</v>
+      </c>
+      <c r="H28">
+        <v>-2.585295462437228E-2</v>
+      </c>
+      <c r="I28">
+        <v>6.9727455013474069</v>
+      </c>
+      <c r="J28">
+        <v>0.95262788465782455</v>
+      </c>
+      <c r="K28">
+        <v>5.3079475912811453</v>
+      </c>
+      <c r="L28">
+        <v>2.717753252477852</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B29">
         <v>1.3181818000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>-3.8846449090330108E-3</v>
+      </c>
+      <c r="D29">
+        <v>8.8464716124400979</v>
+      </c>
+      <c r="E29">
+        <v>-0.26350578807786101</v>
+      </c>
+      <c r="F29">
+        <v>1.0036556491243389</v>
+      </c>
+      <c r="G29">
+        <v>2.9891263633021792</v>
+      </c>
+      <c r="H29">
+        <v>7.4943800883418062E-3</v>
+      </c>
+      <c r="I29">
+        <v>5.4960963292080729</v>
+      </c>
+      <c r="J29">
+        <v>0.79932922362463465</v>
+      </c>
+      <c r="K29">
+        <v>4.8722610874177468</v>
+      </c>
+      <c r="L29">
+        <v>3.3725629551396952</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B30">
         <v>1.3636364000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>-0.38570867585723823</v>
+      </c>
+      <c r="D30">
+        <v>6.2875298123464756</v>
+      </c>
+      <c r="E30">
+        <v>0.34755054856389972</v>
+      </c>
+      <c r="F30">
+        <v>1.020557754404535</v>
+      </c>
+      <c r="G30">
+        <v>2.9675074575052132</v>
+      </c>
+      <c r="H30">
+        <v>-0.21030509959463711</v>
+      </c>
+      <c r="I30">
+        <v>6.9829381477057986</v>
+      </c>
+      <c r="J30">
+        <v>1.1843875833120869</v>
+      </c>
+      <c r="K30">
+        <v>5.3744424779977216</v>
+      </c>
+      <c r="L30">
+        <v>4.2032007001294858</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B31">
         <v>1.2727272999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>-0.28365646339959261</v>
+      </c>
+      <c r="D31">
+        <v>8.4761573168539055</v>
+      </c>
+      <c r="E31">
+        <v>0.3225175750772265</v>
+      </c>
+      <c r="F31">
+        <v>1.0224846374360319</v>
+      </c>
+      <c r="G31">
+        <v>3.5713616660186149</v>
+      </c>
+      <c r="H31">
+        <v>-0.68643204493776844</v>
+      </c>
+      <c r="I31">
+        <v>6.7025293878828016</v>
+      </c>
+      <c r="J31">
+        <v>1.1052769037023089</v>
+      </c>
+      <c r="K31">
+        <v>4.6732679219463069</v>
+      </c>
+      <c r="L31">
+        <v>3.8317322959166722</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B32">
         <v>1.0454545</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>3.7521081187250038</v>
+      </c>
+      <c r="D32">
+        <v>4.8258915598826677</v>
+      </c>
+      <c r="E32">
+        <v>4.5023294530540134</v>
+      </c>
+      <c r="F32">
+        <v>0.65372611953308568</v>
+      </c>
+      <c r="G32">
+        <v>4.1939307633832392</v>
+      </c>
+      <c r="H32">
+        <v>0.99210217491123698</v>
+      </c>
+      <c r="I32">
+        <v>4.6740414641302506</v>
+      </c>
+      <c r="J32">
+        <v>9.1827649207712012E-2</v>
+      </c>
+      <c r="K32">
+        <v>1.7125346095728731</v>
+      </c>
+      <c r="L32">
+        <v>3.951716500617608</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <v>1.2272727000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>3.5980183405427089</v>
+      </c>
+      <c r="D33">
+        <v>3.4775839006134688</v>
+      </c>
+      <c r="E33">
+        <v>4.4945257627987232</v>
+      </c>
+      <c r="F33">
+        <v>0.36648711637667442</v>
+      </c>
+      <c r="G33">
+        <v>3.8757525593387392</v>
+      </c>
+      <c r="H33">
+        <v>0.76370844893204548</v>
+      </c>
+      <c r="I33">
+        <v>4.1556244625013958</v>
+      </c>
+      <c r="J33">
+        <v>0.53349636512461307</v>
+      </c>
+      <c r="K33">
+        <v>1.855611356695996</v>
+      </c>
+      <c r="L33">
+        <v>4.083037603117627</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B34">
         <v>1.2727272999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>3.0244740184161079</v>
+      </c>
+      <c r="D34">
+        <v>3.975018773442994</v>
+      </c>
+      <c r="E34">
+        <v>5.0585446031983254</v>
+      </c>
+      <c r="F34">
+        <v>0.62830293020347383</v>
+      </c>
+      <c r="G34">
+        <v>4.4373628825434022</v>
+      </c>
+      <c r="H34">
+        <v>0.70834267510343807</v>
+      </c>
+      <c r="I34">
+        <v>4.2749263778669553</v>
+      </c>
+      <c r="J34">
+        <v>0.45183623646289389</v>
+      </c>
+      <c r="K34">
+        <v>2.2513744227045658</v>
+      </c>
+      <c r="L34">
+        <v>3.9785888057173251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B35">
         <v>1.2727272999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>4.0106971935203948</v>
+      </c>
+      <c r="D35">
+        <v>4.8151494603135259</v>
+      </c>
+      <c r="E35">
+        <v>4.8457056907297202</v>
+      </c>
+      <c r="F35">
+        <v>0.58965099343193528</v>
+      </c>
+      <c r="G35">
+        <v>4.1457165667627676</v>
+      </c>
+      <c r="H35">
+        <v>0.90356277778914607</v>
+      </c>
+      <c r="I35">
+        <v>3.8936865355799331</v>
+      </c>
+      <c r="J35">
+        <v>-0.40091226299775717</v>
+      </c>
+      <c r="K35">
+        <v>2.1405107086050279</v>
+      </c>
+      <c r="L35">
+        <v>4.0558205228575996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B36">
         <v>1.3636364000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>3.688718875544633</v>
+      </c>
+      <c r="D36">
+        <v>3.914696471497896</v>
+      </c>
+      <c r="E36">
+        <v>4.898006295747507</v>
+      </c>
+      <c r="F36">
+        <v>0.48945058959256188</v>
+      </c>
+      <c r="G36">
+        <v>3.964652395565762</v>
+      </c>
+      <c r="H36">
+        <v>1.0073583739637919</v>
+      </c>
+      <c r="I36">
+        <v>3.392145317028993</v>
+      </c>
+      <c r="J36">
+        <v>0.225552015505771</v>
+      </c>
+      <c r="K36">
+        <v>2.0928283819601639</v>
+      </c>
+      <c r="L36">
+        <v>4.3321778728418359</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B37">
         <v>1.3863635999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>3.3536296808469781</v>
+      </c>
+      <c r="D37">
+        <v>3.5558996710784818</v>
+      </c>
+      <c r="E37">
+        <v>6.2180137571847283</v>
+      </c>
+      <c r="F37">
+        <v>0.70527005161674794</v>
+      </c>
+      <c r="G37">
+        <v>4.1584210341521306</v>
+      </c>
+      <c r="H37">
+        <v>0.97242573267374766</v>
+      </c>
+      <c r="I37">
+        <v>4.148003883823157</v>
+      </c>
+      <c r="J37">
+        <v>-0.1005017231269265</v>
+      </c>
+      <c r="K37">
+        <v>2.148107900724332</v>
+      </c>
+      <c r="L37">
+        <v>3.854945544299555</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B38">
         <v>1.7954545</v>
+      </c>
+      <c r="C38">
+        <v>4.2062983113022874</v>
+      </c>
+      <c r="D38">
+        <v>4.9356967601753432</v>
+      </c>
+      <c r="E38">
+        <v>3.9337506293760409</v>
+      </c>
+      <c r="F38">
+        <v>0.46323522763219133</v>
+      </c>
+      <c r="G38">
+        <v>3.9353689736525048</v>
+      </c>
+      <c r="H38">
+        <v>1.0189357592300221</v>
+      </c>
+      <c r="I38">
+        <v>4.3001673037331507</v>
+      </c>
+      <c r="J38">
+        <v>-7.0809627318162462E-3</v>
+      </c>
+      <c r="K38">
+        <v>1.797425143982905</v>
+      </c>
+      <c r="L38">
+        <v>4.4062460043286276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>